<commit_message>
Industry balances multiple factories for single and multiple scenarios
</commit_message>
<xml_diff>
--- a/excelData/cementIndustry.xlsx
+++ b/excelData/cementIndustry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E2C204D3-A32C-A943-8377-06CFBF6D5DC5}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F46DAC1-6590-F34E-8A1A-5D08999055C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="4100" yWindow="520" windowWidth="25260" windowHeight="17400" activeTab="1" xr2:uid="{6BDE4EC1-0576-1041-BEA7-94E25ADD72B4}"/>
+    <workbookView xWindow="3540" yWindow="520" windowWidth="25260" windowHeight="17400" activeTab="4" xr2:uid="{6BDE4EC1-0576-1041-BEA7-94E25ADD72B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Factory List" sheetId="1" r:id="rId1"/>
@@ -18,7 +18,7 @@
     <sheet name="2010-Absolute" sheetId="5" r:id="rId3"/>
     <sheet name="1990-Relative" sheetId="7" r:id="rId4"/>
     <sheet name="2010-Relative" sheetId="8" r:id="rId5"/>
-    <sheet name="1990-2010" sheetId="6" r:id="rId6"/>
+    <sheet name="1990-2010-Growth" sheetId="6" r:id="rId6"/>
   </sheets>
   <calcPr calcId="162913"/>
   <extLst>
@@ -30,7 +30,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="102" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="31">
   <si>
     <t>Factory Name</t>
   </si>
@@ -99,6 +99,30 @@
   </si>
   <si>
     <t>industry</t>
+  </si>
+  <si>
+    <t>blenderFactory</t>
+  </si>
+  <si>
+    <t>same_cement</t>
+  </si>
+  <si>
+    <t>excelData/cementFactory.xlsx</t>
+  </si>
+  <si>
+    <t>excelData/otherCementFactory.xlsx</t>
+  </si>
+  <si>
+    <t>excelData/clinkerFactory.xlsx</t>
+  </si>
+  <si>
+    <t>excelData/blenderFactory.xlsx</t>
+  </si>
+  <si>
+    <t>Chain List</t>
+  </si>
+  <si>
+    <t>Connections</t>
   </si>
 </sst>
 </file>
@@ -450,10 +474,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{175EC475-3700-0947-86B4-662169F58206}">
-  <dimension ref="A1:D5"/>
+  <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -482,20 +506,70 @@
       <c r="A2" t="s">
         <v>1</v>
       </c>
+      <c r="B2" t="s">
+        <v>25</v>
+      </c>
+      <c r="C2" t="s">
+        <v>29</v>
+      </c>
+      <c r="D2" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>14</v>
       </c>
+      <c r="B3" t="s">
+        <v>25</v>
+      </c>
+      <c r="C3" t="s">
+        <v>29</v>
+      </c>
+      <c r="D3" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>2</v>
       </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>29</v>
+      </c>
+      <c r="D4" t="s">
+        <v>30</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>18</v>
+      </c>
+      <c r="B5" t="s">
+        <v>27</v>
+      </c>
+      <c r="C5" t="s">
+        <v>29</v>
+      </c>
+      <c r="D5" t="s">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>28</v>
+      </c>
+      <c r="C6" t="s">
+        <v>29</v>
+      </c>
+      <c r="D6" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
@@ -507,8 +581,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6CBBB1-E2E4-CC4B-8796-B164A9C9EFB5}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B33" sqref="B33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C33" sqref="C33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -565,7 +639,7 @@
         <v>14</v>
       </c>
       <c r="B4" t="s">
-        <v>9</v>
+        <v>24</v>
       </c>
       <c r="C4">
         <v>500</v>
@@ -687,7 +761,7 @@
   <dimension ref="A1:D6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B2" sqref="A2:B2"/>
+      <selection activeCell="G38" sqref="G38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -787,8 +861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE746189-6A36-404D-ADC0-B082F679DA50}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="C12" sqref="C12"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -899,7 +973,7 @@
   <dimension ref="A1:H5"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="J34" sqref="J34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
industry.evolve now works for linear scenarios
Industry.evolve linearly calculates annual and cumulative input and output given start and stop years.
</commit_message>
<xml_diff>
--- a/excelData/cementIndustry.xlsx
+++ b/excelData/cementIndustry.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/Tanzer/GitHub/BlackBlox/excelData/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6F46DAC1-6590-F34E-8A1A-5D08999055C7}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3A75DEDC-6261-2B4E-996A-247EF7E84CA8}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3540" yWindow="520" windowWidth="25260" windowHeight="17400" activeTab="4" xr2:uid="{6BDE4EC1-0576-1041-BEA7-94E25ADD72B4}"/>
+    <workbookView xWindow="3540" yWindow="520" windowWidth="25260" windowHeight="17400" activeTab="2" xr2:uid="{6BDE4EC1-0576-1041-BEA7-94E25ADD72B4}"/>
   </bookViews>
   <sheets>
     <sheet name="Factory List" sheetId="1" r:id="rId1"/>
@@ -671,8 +671,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{464CAE28-609C-4242-8DBB-9F5FE71AC790}">
   <dimension ref="A1:D5"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G40" sqref="G40"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C19" sqref="C19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -703,7 +703,7 @@
         <v>9</v>
       </c>
       <c r="C2">
-        <v>400</v>
+        <v>1000</v>
       </c>
       <c r="D2" t="s">
         <v>10</v>
@@ -717,7 +717,7 @@
         <v>9</v>
       </c>
       <c r="C3">
-        <v>400</v>
+        <v>600</v>
       </c>
       <c r="D3" t="s">
         <v>16</v>
@@ -745,7 +745,7 @@
         <v>19</v>
       </c>
       <c r="C5">
-        <v>80</v>
+        <v>0</v>
       </c>
       <c r="D5" t="s">
         <v>10</v>
@@ -861,7 +861,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{DE746189-6A36-404D-ADC0-B082F679DA50}">
   <dimension ref="A1:D7"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D7" sqref="D7"/>
     </sheetView>
   </sheetViews>

</xml_diff>